<commit_message>
more modularity in the belongingnes and ST inclusion or exclusion
</commit_message>
<xml_diff>
--- a/data/Dr Challoners Data/IBSC Teacher Dr Challoners 10F.xlsx
+++ b/data/Dr Challoners Data/IBSC Teacher Dr Challoners 10F.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c85ca06803d405f/2017-2019/Documents/RF/IBSC Survey Feedback/Master Dash/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c85ca06803d405f/2017-2019/Documents/RF/IBSC Survey Feedback/Master Dash/data/Dr Challoners Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_464F48C1FD0C5AB06E6A1E2BD416CE75CF73FC5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5DA9F6-D27A-4EDC-AFED-D607DB7B1E3A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_464F48C1FD0C5AB06E6A1E2BD416CE75CF73FC5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F6FB556-5D53-41EE-9261-9E81F6F83449}"/>
   <bookViews>
-    <workbookView xWindow="43740" yWindow="2390" windowWidth="28100" windowHeight="15910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Attributes" sheetId="1" r:id="rId1"/>
@@ -1002,6 +1002,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>